<commit_message>
Add fake data for database
</commit_message>
<xml_diff>
--- a/cups_db.xlsx
+++ b/cups_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F33D82-41D3-455B-8FD8-BA9DB8E22E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6795050A-771C-4092-82E0-F01389876A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55055081-DE6E-4B45-951F-D4AB37DE9E6F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="12">
   <si>
     <t>cup_id</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>SB3</t>
+  </si>
+  <si>
+    <t>Out</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617DB90-6D3E-464D-87D2-F756CC04DABA}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B16" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -467,7 +473,7 @@
         <v>989966</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -481,12 +487,180 @@
         <v>989967</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>989968</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>989969</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>989970</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>989971</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>989972</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>989973</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>989974</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>989975</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>989976</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>989977</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>989978</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>989979</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>